<commit_message>
Updated metadata file to clarify merchant id
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CP318189\Documents\Repos\data-science-challenge\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CP348682\Desktop\TEMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7464"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Merchant identifier to separate different businesses. </t>
-  </si>
-  <si>
     <t>Date on which transaction occurred.</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t xml:space="preserve">Postal code of town/city of business. </t>
   </si>
   <si>
-    <t xml:space="preserve">Generic name of merchant, this also shows where </t>
-  </si>
-  <si>
     <t xml:space="preserve">Age band of client who did transaction. </t>
   </si>
   <si>
@@ -126,6 +120,12 @@
   </si>
   <si>
     <t>Avg_Income_3M</t>
+  </si>
+  <si>
+    <t>Merchant ID, but could be of separate stores, use Merchant_name as unique Merchant identifier</t>
+  </si>
+  <si>
+    <t>Generic name of merchant, should be used as unique business identifier.</t>
   </si>
 </sst>
 </file>
@@ -447,16 +447,16 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -464,132 +464,132 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>